<commit_message>
QAPF with Result Report and Index Showing
</commit_message>
<xml_diff>
--- a/NodeSamples/测试节点/Clastic.xlsx
+++ b/NodeSamples/测试节点/Clastic.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fred\Documents\GitHub\GeoPyTool\NodeSamples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\GeoPyTool\NodeSamples\测试节点\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401BF642-DDF1-452E-85DE-92C80EC5B6C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961A352A-9491-4535-9AD3-E1ABF3BD047A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10290" yWindow="4395" windowWidth="12255" windowHeight="15060" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3660" yWindow="555" windowWidth="21600" windowHeight="16200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="你的数据" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="222">
   <si>
     <t>﻿Suites</t>
   </si>
@@ -719,23 +719,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>green</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Index</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>red</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>顶点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grey</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1345,10 +1345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -1361,7 +1361,7 @@
         <v>207</v>
       </c>
       <c r="B1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>209</v>
@@ -1412,13 +1412,13 @@
         <v>182</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>183</v>
+        <v>221</v>
       </c>
       <c r="H2" s="2">
         <v>50</v>
       </c>
       <c r="I2" s="2">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>184</v>
@@ -1448,13 +1448,13 @@
         <v>182</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>183</v>
+        <v>221</v>
       </c>
       <c r="H3" s="2">
         <v>50</v>
       </c>
       <c r="I3" s="2">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>184</v>
@@ -1484,13 +1484,13 @@
         <v>182</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>183</v>
+        <v>221</v>
       </c>
       <c r="H4" s="2">
         <v>50</v>
       </c>
       <c r="I4" s="2">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>184</v>
@@ -1520,13 +1520,13 @@
         <v>182</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>183</v>
+        <v>221</v>
       </c>
       <c r="H5" s="2">
         <v>50</v>
       </c>
       <c r="I5" s="2">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>184</v>
@@ -1556,13 +1556,13 @@
         <v>182</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>183</v>
+        <v>221</v>
       </c>
       <c r="H6" s="2">
         <v>50</v>
       </c>
       <c r="I6" s="2">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>184</v>
@@ -1592,13 +1592,13 @@
         <v>182</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="H7" s="2">
         <v>50</v>
       </c>
       <c r="I7" s="2">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>184</v>
@@ -1628,13 +1628,13 @@
         <v>182</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="H8" s="2">
         <v>50</v>
       </c>
       <c r="I8" s="2">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>184</v>
@@ -1664,13 +1664,13 @@
         <v>182</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="H9" s="2">
         <v>50</v>
       </c>
       <c r="I9" s="2">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>184</v>
@@ -1700,13 +1700,13 @@
         <v>182</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="H10" s="2">
         <v>50</v>
       </c>
       <c r="I10" s="2">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>184</v>
@@ -1736,13 +1736,13 @@
         <v>182</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="H11" s="2">
         <v>50</v>
       </c>
       <c r="I11" s="2">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>184</v>
@@ -1772,13 +1772,13 @@
         <v>182</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="H12" s="2">
         <v>50</v>
       </c>
       <c r="I12" s="2">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>184</v>
@@ -1808,13 +1808,13 @@
         <v>182</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="H13" s="2">
         <v>50</v>
       </c>
       <c r="I13" s="2">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>184</v>
@@ -1844,13 +1844,13 @@
         <v>182</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="H14" s="2">
         <v>50</v>
       </c>
       <c r="I14" s="2">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>184</v>
@@ -1879,13 +1879,13 @@
         <v>182</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="H15" s="2">
         <v>50</v>
       </c>
       <c r="I15" s="2">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>184</v>
@@ -1914,13 +1914,13 @@
         <v>182</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="H16" s="2">
         <v>50</v>
       </c>
       <c r="I16" s="2">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>184</v>
@@ -1949,13 +1949,13 @@
         <v>182</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="H17" s="2">
         <v>50</v>
       </c>
       <c r="I17" s="2">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>184</v>
@@ -1984,13 +1984,13 @@
         <v>182</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="H18" s="2">
         <v>50</v>
       </c>
       <c r="I18" s="2">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>184</v>
@@ -2019,18 +2019,123 @@
         <v>182</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="H19" s="2">
         <v>50</v>
       </c>
       <c r="I19" s="2">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>184</v>
       </c>
       <c r="K19" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" s="14">
+        <v>0</v>
+      </c>
+      <c r="D20" s="14">
+        <v>0</v>
+      </c>
+      <c r="E20" s="14">
+        <v>100</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="H20" s="2">
+        <v>50</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="K20" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" s="14">
+        <v>0</v>
+      </c>
+      <c r="D21" s="14">
+        <v>100</v>
+      </c>
+      <c r="E21" s="14">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="H21" s="2">
+        <v>50</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="K21" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" s="14">
+        <v>100</v>
+      </c>
+      <c r="D22" s="14">
+        <v>0</v>
+      </c>
+      <c r="E22" s="14">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="H22" s="2">
+        <v>50</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="K22" s="2">
         <v>0.4</v>
       </c>
     </row>
@@ -2045,7 +2150,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91203CB7-7716-41B8-B27A-CEE68F0EBCB7}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1:F18"/>
     </sheetView>
   </sheetViews>
@@ -2056,7 +2161,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C1" s="14">
         <v>50</v>
@@ -2068,7 +2173,7 @@
         <v>50</v>
       </c>
       <c r="F1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2076,7 +2181,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C2" s="14">
         <v>40</v>
@@ -2088,7 +2193,7 @@
         <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2096,7 +2201,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C3" s="14">
         <v>0</v>
@@ -2108,7 +2213,7 @@
         <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2116,7 +2221,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C4" s="14">
         <v>20</v>
@@ -2128,7 +2233,7 @@
         <v>40</v>
       </c>
       <c r="F4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2136,7 +2241,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C5" s="14">
         <v>50</v>
@@ -2148,7 +2253,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2156,7 +2261,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C6" s="14">
         <v>40</v>
@@ -2168,7 +2273,7 @@
         <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2176,7 +2281,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C7" s="14">
         <v>25</v>
@@ -2188,7 +2293,7 @@
         <v>75</v>
       </c>
       <c r="F7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2196,7 +2301,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C8" s="14">
         <v>0</v>
@@ -2208,7 +2313,7 @@
         <v>75</v>
       </c>
       <c r="F8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2216,7 +2321,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C9" s="14">
         <v>75</v>
@@ -2228,7 +2333,7 @@
         <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2236,7 +2341,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C10" s="14">
         <v>75</v>
@@ -2248,7 +2353,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2256,7 +2361,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C11" s="14">
         <v>25</v>
@@ -2268,7 +2373,7 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2276,7 +2381,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C12" s="14">
         <v>0</v>
@@ -2288,7 +2393,7 @@
         <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2296,7 +2401,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C13" s="14">
         <v>20</v>
@@ -2308,7 +2413,7 @@
         <v>60</v>
       </c>
       <c r="F13" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2316,7 +2421,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C14" s="14">
         <v>60</v>
@@ -2328,7 +2433,7 @@
         <v>20</v>
       </c>
       <c r="F14" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2336,7 +2441,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C15" s="14">
         <v>20</v>
@@ -2348,7 +2453,7 @@
         <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2356,7 +2461,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C16" s="14">
         <v>12.5</v>
@@ -2368,7 +2473,7 @@
         <v>75</v>
       </c>
       <c r="F16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2376,7 +2481,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C17" s="14">
         <v>75</v>
@@ -2388,7 +2493,7 @@
         <v>12.5</v>
       </c>
       <c r="F17" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2396,7 +2501,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C18" s="14">
         <v>12.5</v>
@@ -2408,7 +2513,7 @@
         <v>12.5</v>
       </c>
       <c r="F18" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -2432,7 +2537,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15">
       <c r="A1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>207</v>

</xml_diff>